<commit_message>
tambah menu crud sub kriteria lowongan
</commit_message>
<xml_diff>
--- a/Data Dummy/perhitungan metode topsis.xlsx
+++ b/Data Dummy/perhitungan metode topsis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BISMILLAH SKRIPSI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BISMILLAH SKRIPSI\Project\SiBuKer_topsis\Data Dummy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,6 +16,7 @@
     <sheet name="TOPSIS" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="95">
   <si>
     <t>Kriteria</t>
   </si>
@@ -292,6 +293,24 @@
   </si>
   <si>
     <t>Kriteria Alumni</t>
+  </si>
+  <si>
+    <t>Keterangan</t>
+  </si>
+  <si>
+    <t>Sangat Tinggi</t>
+  </si>
+  <si>
+    <t>Tinggi</t>
+  </si>
+  <si>
+    <t>Cukup</t>
+  </si>
+  <si>
+    <t>Rendah</t>
+  </si>
+  <si>
+    <t>Sangat Rendah</t>
   </si>
 </sst>
 </file>
@@ -612,7 +631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -888,6 +907,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1972,8 +1997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X33" sqref="X33"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2367,6 +2392,12 @@
         <v>88</v>
       </c>
       <c r="Q10" s="26"/>
+      <c r="R10" s="106" t="s">
+        <v>8</v>
+      </c>
+      <c r="S10" s="107" t="s">
+        <v>89</v>
+      </c>
       <c r="V10" s="97"/>
       <c r="W10" s="8" t="s">
         <v>29</v>
@@ -2384,6 +2415,12 @@
       <c r="F11" s="54"/>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
+      <c r="R11" s="106">
+        <v>5</v>
+      </c>
+      <c r="S11" s="106" t="s">
+        <v>90</v>
+      </c>
       <c r="V11" s="97"/>
       <c r="W11" s="69" t="s">
         <v>45</v>
@@ -2399,6 +2436,12 @@
       <c r="B12" s="100"/>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
+      <c r="R12" s="106">
+        <v>4</v>
+      </c>
+      <c r="S12" s="106" t="s">
+        <v>91</v>
+      </c>
       <c r="V12" s="96" t="s">
         <v>42</v>
       </c>
@@ -2427,6 +2470,12 @@
       </c>
       <c r="G13" s="67" t="s">
         <v>60</v>
+      </c>
+      <c r="R13" s="106">
+        <v>3</v>
+      </c>
+      <c r="S13" s="106" t="s">
+        <v>92</v>
       </c>
       <c r="V13" s="96"/>
       <c r="W13" s="85" t="s">
@@ -2464,6 +2513,12 @@
         <f>G3/N3</f>
         <v>0.44721359549995793</v>
       </c>
+      <c r="R14" s="106">
+        <v>2</v>
+      </c>
+      <c r="S14" s="106" t="s">
+        <v>93</v>
+      </c>
       <c r="V14" s="96"/>
       <c r="W14" s="85" t="s">
         <v>51</v>
@@ -2499,6 +2554,12 @@
       <c r="G15" s="81">
         <f>G4/N3</f>
         <v>0.44721359549995793</v>
+      </c>
+      <c r="R15" s="106">
+        <v>1</v>
+      </c>
+      <c r="S15" s="106" t="s">
+        <v>94</v>
       </c>
       <c r="V15" s="96"/>
       <c r="W15" s="85" t="s">
@@ -3361,6 +3422,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A39:M39"/>
+    <mergeCell ref="A48:M48"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="I9:N9"/>
     <mergeCell ref="V19:V22"/>
     <mergeCell ref="V24:V33"/>
     <mergeCell ref="R2:T2"/>
@@ -3368,11 +3434,6 @@
     <mergeCell ref="V7:V11"/>
     <mergeCell ref="V12:V15"/>
     <mergeCell ref="V16:V18"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A39:M39"/>
-    <mergeCell ref="A48:M48"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="I9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>